<commit_message>
API Data Type, Type conversion, DateTime
</commit_message>
<xml_diff>
--- a/API/API_BasicTraining.xlsx
+++ b/API/API_BasicTraining.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="80">
   <si>
     <t>No</t>
   </si>
@@ -268,6 +268,15 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>17-8-23</t>
+  </si>
+  <si>
+    <t>19-8-23</t>
+  </si>
+  <si>
+    <t>21-8-23</t>
   </si>
 </sst>
 </file>
@@ -407,7 +416,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -427,6 +436,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -438,15 +462,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -734,15 +749,18 @@
   <dimension ref="A1:G94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:E16"/>
+      <selection activeCell="F5" sqref="F5:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -761,7 +779,7 @@
       <c r="E1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>75</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -780,8 +798,8 @@
         <v>6</v>
       </c>
       <c r="E2" s="7"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="5"/>
@@ -793,8 +811,12 @@
       <c r="E3" s="7">
         <v>1</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="F3" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="5"/>
@@ -808,8 +830,8 @@
         <v>10</v>
       </c>
       <c r="E4" s="7"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="5"/>
@@ -822,11 +844,15 @@
       <c r="D5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="15">
         <v>2</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="5"/>
@@ -835,9 +861,9 @@
       <c r="D6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="5"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="5"/>
@@ -846,9 +872,9 @@
       <c r="D7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="5"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="13"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="5"/>
@@ -860,8 +886,12 @@
       <c r="E8" s="7">
         <v>1</v>
       </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="F8" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="5"/>
@@ -870,11 +900,15 @@
       <c r="D9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="15">
         <v>1</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="F9" s="15">
+        <v>0.75</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="5"/>
@@ -883,9 +917,9 @@
       <c r="D10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="5"/>
@@ -894,9 +928,9 @@
       <c r="D11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="5"/>
@@ -905,11 +939,11 @@
       <c r="D12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="15">
         <v>2</v>
       </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="5"/>
@@ -918,9 +952,9 @@
       <c r="D13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="5"/>
@@ -929,11 +963,11 @@
       <c r="D14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="15">
         <v>4</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="5"/>
@@ -942,9 +976,9 @@
       <c r="D15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="5"/>
@@ -953,9 +987,9 @@
       <c r="D16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="5"/>
@@ -967,8 +1001,8 @@
       <c r="E17" s="7">
         <v>2</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="5"/>
@@ -977,9 +1011,11 @@
       <c r="D18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="E18" s="7">
+        <v>1</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="5"/>
@@ -988,9 +1024,11 @@
       <c r="D19" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="E19" s="7">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="9"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="5"/>
@@ -999,9 +1037,11 @@
       <c r="D20" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="E20" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="9"/>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="5"/>
@@ -1011,8 +1051,8 @@
         <v>29</v>
       </c>
       <c r="E21" s="7"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="9"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="5"/>
@@ -1022,8 +1062,8 @@
         <v>30</v>
       </c>
       <c r="E22" s="7"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="9"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="5"/>
@@ -1033,8 +1073,8 @@
         <v>31</v>
       </c>
       <c r="E23" s="7"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="9"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="5"/>
@@ -1044,8 +1084,8 @@
         <v>32</v>
       </c>
       <c r="E24" s="7"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="9"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="5"/>
@@ -1055,8 +1095,8 @@
         <v>33</v>
       </c>
       <c r="E25" s="7"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="9"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="5"/>
@@ -1066,8 +1106,8 @@
         <v>34</v>
       </c>
       <c r="E26" s="7"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="9"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="5"/>
@@ -1077,8 +1117,8 @@
         <v>35</v>
       </c>
       <c r="E27" s="7"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="9"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="5"/>
@@ -1088,8 +1128,8 @@
         <v>36</v>
       </c>
       <c r="E28" s="7"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="9"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="5"/>
@@ -1099,8 +1139,8 @@
         <v>37</v>
       </c>
       <c r="E29" s="7"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="5"/>
@@ -1108,8 +1148,8 @@
       <c r="C30" s="2"/>
       <c r="D30" s="5"/>
       <c r="E30" s="7"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="9"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="5"/>
@@ -1117,8 +1157,8 @@
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="7"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="9"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="5"/>
@@ -1126,21 +1166,21 @@
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="7"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="9"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="5"/>
       <c r="B33" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="9"/>
+      <c r="D33" s="14"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="9"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="5"/>
@@ -1152,8 +1192,8 @@
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="7"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="9"/>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="5"/>
@@ -1167,8 +1207,8 @@
         <v>44</v>
       </c>
       <c r="E35" s="7"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="9"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="5"/>
@@ -1178,8 +1218,8 @@
         <v>45</v>
       </c>
       <c r="E36" s="7"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="9"/>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="5"/>
@@ -1189,8 +1229,8 @@
         <v>46</v>
       </c>
       <c r="E37" s="7"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="9"/>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="5"/>
@@ -1200,8 +1240,8 @@
         <v>47</v>
       </c>
       <c r="E38" s="7"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="9"/>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="5"/>
@@ -1211,8 +1251,8 @@
         <v>48</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="9"/>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="5"/>
@@ -1222,8 +1262,8 @@
         <v>49</v>
       </c>
       <c r="E40" s="7"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="9"/>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="5"/>
@@ -1233,8 +1273,8 @@
         <v>50</v>
       </c>
       <c r="E41" s="7"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="9"/>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="5"/>
@@ -1244,8 +1284,8 @@
         <v>51</v>
       </c>
       <c r="E42" s="7"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="9"/>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="5"/>
@@ -1255,8 +1295,8 @@
         <v>52</v>
       </c>
       <c r="E43" s="7"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="9"/>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="5"/>
@@ -1266,8 +1306,8 @@
         <v>53</v>
       </c>
       <c r="E44" s="7"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="9"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="5"/>
@@ -1277,8 +1317,8 @@
         <v>54</v>
       </c>
       <c r="E45" s="7"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="9"/>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="5"/>
@@ -1288,8 +1328,8 @@
         <v>55</v>
       </c>
       <c r="E46" s="7"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="9"/>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="5"/>
@@ -1299,8 +1339,8 @@
         <v>56</v>
       </c>
       <c r="E47" s="7"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="9"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="5"/>
@@ -1310,8 +1350,8 @@
         <v>57</v>
       </c>
       <c r="E48" s="7"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="9"/>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="5"/>
@@ -1321,8 +1361,8 @@
         <v>58</v>
       </c>
       <c r="E49" s="7"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="9"/>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="5"/>
@@ -1332,8 +1372,8 @@
         <v>59</v>
       </c>
       <c r="E50" s="7"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="9"/>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="5"/>
@@ -1343,8 +1383,8 @@
         <v>60</v>
       </c>
       <c r="E51" s="7"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="9"/>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="5"/>
@@ -1352,8 +1392,8 @@
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="7"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="9"/>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="5"/>
@@ -1361,21 +1401,21 @@
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="7"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="9"/>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="5"/>
       <c r="B54" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C54" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D54" s="9"/>
+      <c r="D54" s="14"/>
       <c r="E54" s="7"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="9"/>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="5"/>
@@ -1383,8 +1423,8 @@
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="7"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="9"/>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="5"/>
@@ -1392,8 +1432,8 @@
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="7"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="9"/>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="5"/>
@@ -1407,8 +1447,8 @@
         <v>35</v>
       </c>
       <c r="E57" s="7"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="9"/>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="5"/>
@@ -1418,8 +1458,8 @@
         <v>36</v>
       </c>
       <c r="E58" s="7"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="9"/>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="5"/>
@@ -1429,8 +1469,8 @@
         <v>37</v>
       </c>
       <c r="E59" s="7"/>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="9"/>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="5"/>
@@ -1440,8 +1480,8 @@
         <v>65</v>
       </c>
       <c r="E60" s="7"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="9"/>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="5"/>
@@ -1451,8 +1491,8 @@
         <v>66</v>
       </c>
       <c r="E61" s="7"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="9"/>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="5"/>
@@ -1462,8 +1502,8 @@
         <v>67</v>
       </c>
       <c r="E62" s="7"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="9"/>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="5"/>
@@ -1473,8 +1513,8 @@
         <v>68</v>
       </c>
       <c r="E63" s="7"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="9"/>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="5"/>
@@ -1484,8 +1524,8 @@
         <v>69</v>
       </c>
       <c r="E64" s="7"/>
-      <c r="F64" s="5"/>
-      <c r="G64" s="5"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="9"/>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" s="5"/>
@@ -1495,8 +1535,8 @@
         <v>70</v>
       </c>
       <c r="E65" s="7"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
+      <c r="F65" s="7"/>
+      <c r="G65" s="9"/>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="5"/>
@@ -1506,8 +1546,8 @@
         <v>71</v>
       </c>
       <c r="E66" s="7"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5"/>
+      <c r="F66" s="7"/>
+      <c r="G66" s="9"/>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="5"/>
@@ -1515,21 +1555,21 @@
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
       <c r="E67" s="7"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="9"/>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="5"/>
       <c r="B68" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C68" s="9" t="s">
+      <c r="C68" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="D68" s="9"/>
+      <c r="D68" s="14"/>
       <c r="E68" s="7"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="5"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="9"/>
     </row>
     <row r="79" spans="1:7">
       <c r="B79" s="1"/>
@@ -1541,7 +1581,8 @@
       <c r="B94" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="11">
+    <mergeCell ref="G5:G7"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C54:D54"/>
     <mergeCell ref="C68:D68"/>
@@ -1550,6 +1591,8 @@
     <mergeCell ref="E9:E11"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="E14:E16"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
C# Demo Of Marksheet Added
</commit_message>
<xml_diff>
--- a/API/API_BasicTraining.xlsx
+++ b/API/API_BasicTraining.xlsx
@@ -748,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
API Demo of Arrays, Functions, Calculator, Value and Reference type Done
</commit_message>
<xml_diff>
--- a/API/API_BasicTraining.xlsx
+++ b/API/API_BasicTraining.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
   <si>
     <t>No</t>
   </si>
@@ -277,6 +277,12 @@
   </si>
   <si>
     <t>21-8-23</t>
+  </si>
+  <si>
+    <t>22-8-23</t>
+  </si>
+  <si>
+    <t>23-8-23</t>
   </si>
 </sst>
 </file>
@@ -748,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:E16"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -942,8 +948,12 @@
       <c r="E12" s="15">
         <v>2</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="9"/>
+      <c r="F12" s="7">
+        <v>1</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="5"/>
@@ -953,8 +963,12 @@
         <v>21</v>
       </c>
       <c r="E13" s="17"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="9"/>
+      <c r="F13" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="5"/>

</xml_diff>

<commit_message>
28 August Work Done
</commit_message>
<xml_diff>
--- a/API/API_BasicTraining.xlsx
+++ b/API/API_BasicTraining.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="83">
   <si>
     <t>No</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>23-8-23</t>
+  </si>
+  <si>
+    <t>24-8-23 &amp; 25-8-23</t>
   </si>
 </sst>
 </file>
@@ -422,7 +425,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -447,6 +450,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -755,7 +767,7 @@
   <dimension ref="A1:G94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -766,7 +778,7 @@
     <col min="4" max="4" width="41.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" style="8" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -850,13 +862,13 @@
       <c r="D5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="18">
         <v>2</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="18">
         <v>1.5</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="14" t="s">
         <v>78</v>
       </c>
     </row>
@@ -867,9 +879,9 @@
       <c r="D6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="12"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="15"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="5"/>
@@ -878,9 +890,9 @@
       <c r="D7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="13"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="16"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="5"/>
@@ -906,13 +918,13 @@
       <c r="D9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="18">
         <v>1</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="18">
         <v>0.75</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="18" t="s">
         <v>79</v>
       </c>
     </row>
@@ -923,9 +935,9 @@
       <c r="D10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="5"/>
@@ -934,9 +946,9 @@
       <c r="D11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="5"/>
@@ -945,7 +957,7 @@
       <c r="D12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="18">
         <v>2</v>
       </c>
       <c r="F12" s="7">
@@ -962,7 +974,7 @@
       <c r="D13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="17"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="7">
         <v>0.75</v>
       </c>
@@ -977,11 +989,15 @@
       <c r="D14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="15">
-        <v>6</v>
-      </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="9"/>
+      <c r="E14" s="11">
+        <v>2</v>
+      </c>
+      <c r="F14" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="5"/>
@@ -990,7 +1006,9 @@
       <c r="D15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="16"/>
+      <c r="E15" s="12">
+        <v>2</v>
+      </c>
       <c r="F15" s="7"/>
       <c r="G15" s="9"/>
     </row>
@@ -1001,7 +1019,9 @@
       <c r="D16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="17"/>
+      <c r="E16" s="13">
+        <v>2</v>
+      </c>
       <c r="F16" s="7"/>
       <c r="G16" s="9"/>
     </row>
@@ -1064,7 +1084,9 @@
       <c r="D21" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="7"/>
+      <c r="E21" s="7">
+        <v>2</v>
+      </c>
       <c r="F21" s="7"/>
       <c r="G21" s="9"/>
     </row>
@@ -1075,7 +1097,9 @@
       <c r="D22" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="7"/>
+      <c r="E22" s="7">
+        <v>2</v>
+      </c>
       <c r="F22" s="7"/>
       <c r="G22" s="9"/>
     </row>
@@ -1086,7 +1110,9 @@
       <c r="D23" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="7"/>
+      <c r="E23" s="7">
+        <v>1</v>
+      </c>
       <c r="F23" s="7"/>
       <c r="G23" s="9"/>
     </row>
@@ -1097,7 +1123,9 @@
       <c r="D24" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="7"/>
+      <c r="E24" s="7">
+        <v>1</v>
+      </c>
       <c r="F24" s="7"/>
       <c r="G24" s="9"/>
     </row>
@@ -1108,7 +1136,9 @@
       <c r="D25" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="7"/>
+      <c r="E25" s="7">
+        <v>1</v>
+      </c>
       <c r="F25" s="7"/>
       <c r="G25" s="9"/>
     </row>
@@ -1119,7 +1149,9 @@
       <c r="D26" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="7"/>
+      <c r="E26" s="7">
+        <v>2</v>
+      </c>
       <c r="F26" s="7"/>
       <c r="G26" s="9"/>
     </row>
@@ -1188,10 +1220,10 @@
       <c r="B33" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="14"/>
+      <c r="D33" s="17"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="9"/>
@@ -1423,10 +1455,10 @@
       <c r="B54" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="C54" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D54" s="14"/>
+      <c r="D54" s="17"/>
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
       <c r="G54" s="9"/>
@@ -1577,10 +1609,10 @@
       <c r="B68" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C68" s="14" t="s">
+      <c r="C68" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="D68" s="14"/>
+      <c r="D68" s="17"/>
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
       <c r="G68" s="9"/>
@@ -1595,7 +1627,7 @@
       <c r="B94" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="10">
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C54:D54"/>
@@ -1604,7 +1636,6 @@
     <mergeCell ref="F5:F7"/>
     <mergeCell ref="E9:E11"/>
     <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E14:E16"/>
     <mergeCell ref="F9:F11"/>
     <mergeCell ref="G9:G11"/>
   </mergeCells>

</xml_diff>

<commit_message>
31 August API Updation
</commit_message>
<xml_diff>
--- a/API/API_BasicTraining.xlsx
+++ b/API/API_BasicTraining.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
   <si>
     <t>No</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>24-8-23 &amp; 25-8-23</t>
+  </si>
+  <si>
+    <t>31-8-23</t>
   </si>
 </sst>
 </file>
@@ -766,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1009,8 +1012,12 @@
       <c r="E15" s="12">
         <v>2</v>
       </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="9"/>
+      <c r="F15" s="7">
+        <v>1</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="5"/>

</xml_diff>

<commit_message>
2 September API Updation
</commit_message>
<xml_diff>
--- a/API/API_BasicTraining.xlsx
+++ b/API/API_BasicTraining.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
   <si>
     <t>No</t>
   </si>
@@ -285,10 +285,22 @@
     <t>23-8-23</t>
   </si>
   <si>
-    <t>24-8-23 &amp; 25-8-23</t>
-  </si>
-  <si>
-    <t>31-8-23</t>
+    <t>1.5 + 1</t>
+  </si>
+  <si>
+    <t>24-8-23 &amp; 25-8-23, 1-9-23</t>
+  </si>
+  <si>
+    <t>1 + 0.5</t>
+  </si>
+  <si>
+    <t>1/9/2023 &amp; 2/9/23</t>
+  </si>
+  <si>
+    <t>1 + 0.75</t>
+  </si>
+  <si>
+    <t>31-8-23 &amp; 2-9-23</t>
   </si>
 </sst>
 </file>
@@ -428,7 +440,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -462,6 +474,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -769,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -781,7 +796,7 @@
     <col min="4" max="4" width="41.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" style="8" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="23" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -865,13 +880,13 @@
       <c r="D5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="19">
         <v>2</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="19">
         <v>1.5</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="15" t="s">
         <v>78</v>
       </c>
     </row>
@@ -882,9 +897,9 @@
       <c r="D6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="15"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="16"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="5"/>
@@ -893,9 +908,9 @@
       <c r="D7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="16"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="5"/>
@@ -921,13 +936,13 @@
       <c r="D9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="19">
         <v>1</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="19">
         <v>0.75</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="19" t="s">
         <v>79</v>
       </c>
     </row>
@@ -938,9 +953,9 @@
       <c r="D10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="5"/>
@@ -949,9 +964,9 @@
       <c r="D11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="5"/>
@@ -960,7 +975,7 @@
       <c r="D12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="19">
         <v>2</v>
       </c>
       <c r="F12" s="7">
@@ -977,7 +992,7 @@
       <c r="D13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="20"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="7">
         <v>0.75</v>
       </c>
@@ -995,11 +1010,11 @@
       <c r="E14" s="11">
         <v>2</v>
       </c>
-      <c r="F14" s="7">
-        <v>1.5</v>
+      <c r="F14" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1012,11 +1027,11 @@
       <c r="E15" s="12">
         <v>2</v>
       </c>
-      <c r="F15" s="7">
-        <v>1</v>
+      <c r="F15" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1029,8 +1044,12 @@
       <c r="E16" s="13">
         <v>2</v>
       </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="9"/>
+      <c r="F16" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="5"/>
@@ -1042,8 +1061,12 @@
       <c r="E17" s="7">
         <v>2</v>
       </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="9"/>
+      <c r="F17" s="7">
+        <v>1</v>
+      </c>
+      <c r="G17" s="14">
+        <v>44966</v>
+      </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="5"/>
@@ -1227,10 +1250,10 @@
       <c r="B33" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C33" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="17"/>
+      <c r="D33" s="18"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="9"/>
@@ -1462,10 +1485,10 @@
       <c r="B54" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C54" s="17" t="s">
+      <c r="C54" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="D54" s="17"/>
+      <c r="D54" s="18"/>
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
       <c r="G54" s="9"/>
@@ -1616,10 +1639,10 @@
       <c r="B68" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C68" s="17" t="s">
+      <c r="C68" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D68" s="17"/>
+      <c r="D68" s="18"/>
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
       <c r="G68" s="9"/>

</xml_diff>

<commit_message>
Part 2 and Test 1 Completed
</commit_message>
<xml_diff>
--- a/API/API_BasicTraining.xlsx
+++ b/API/API_BasicTraining.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="101">
   <si>
     <t>No</t>
   </si>
@@ -319,6 +319,27 @@
   </si>
   <si>
     <t>17-9-23</t>
+  </si>
+  <si>
+    <t>17-10-23</t>
+  </si>
+  <si>
+    <t>2 + 2</t>
+  </si>
+  <si>
+    <t>18-10-23 &amp; 19-10-23</t>
+  </si>
+  <si>
+    <t>2 + 1 + 2</t>
+  </si>
+  <si>
+    <t>20-10-23 &amp; 21-10-23 &amp; 24-10-23</t>
+  </si>
+  <si>
+    <t>3 + 2</t>
+  </si>
+  <si>
+    <t>28-10-23 &amp; 29-10-23</t>
   </si>
 </sst>
 </file>
@@ -803,7 +824,7 @@
   <dimension ref="A1:G94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -814,7 +835,7 @@
     <col min="4" max="4" width="41.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" style="8" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="27" style="10" customWidth="1"/>
+    <col min="7" max="7" width="28.5703125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1246,9 +1267,15 @@
       <c r="D27" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="9"/>
+      <c r="E27" s="7">
+        <v>3</v>
+      </c>
+      <c r="F27" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="5"/>
@@ -1257,9 +1284,15 @@
       <c r="D28" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="9"/>
+      <c r="E28" s="7">
+        <v>5</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="5"/>
@@ -1268,9 +1301,15 @@
       <c r="D29" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="9"/>
+      <c r="E29" s="7">
+        <v>6</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="5"/>
@@ -1308,9 +1347,15 @@
         <v>39</v>
       </c>
       <c r="D33" s="18"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="9"/>
+      <c r="E33" s="7">
+        <v>8</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="5"/>

</xml_diff>

<commit_message>
Till 6th November SQL and API Training Completed Files
</commit_message>
<xml_diff>
--- a/API/API_BasicTraining.xlsx
+++ b/API/API_BasicTraining.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="102">
   <si>
     <t>No</t>
   </si>
@@ -336,10 +336,13 @@
     <t>20-10-23 &amp; 21-10-23 &amp; 24-10-23</t>
   </si>
   <si>
-    <t>3 + 2</t>
-  </si>
-  <si>
-    <t>28-10-23 &amp; 29-10-23</t>
+    <t>3 + 2 + 1.5</t>
+  </si>
+  <si>
+    <t>28-10-23 to 30-10-23</t>
+  </si>
+  <si>
+    <t>3/11/023</t>
   </si>
 </sst>
 </file>
@@ -823,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1381,9 +1384,15 @@
       <c r="D35" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="9"/>
+      <c r="E35" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="F35" s="7">
+        <v>1</v>
+      </c>
+      <c r="G35" s="14">
+        <v>44937</v>
+      </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="5"/>
@@ -1392,9 +1401,15 @@
       <c r="D36" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="9"/>
+      <c r="E36" s="7">
+        <v>1</v>
+      </c>
+      <c r="F36" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="G36" s="14">
+        <v>44937</v>
+      </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="5"/>
@@ -1403,9 +1418,15 @@
       <c r="D37" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="9"/>
+      <c r="E37" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="F37" s="7">
+        <v>1</v>
+      </c>
+      <c r="G37" s="14">
+        <v>44968</v>
+      </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="5"/>
@@ -1414,9 +1435,15 @@
       <c r="D38" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="9"/>
+      <c r="E38" s="7">
+        <v>2</v>
+      </c>
+      <c r="F38" s="7">
+        <v>1</v>
+      </c>
+      <c r="G38" s="14">
+        <v>45057</v>
+      </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="5"/>
@@ -1425,9 +1452,15 @@
       <c r="D39" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="9"/>
+      <c r="E39" s="7">
+        <v>2</v>
+      </c>
+      <c r="F39" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="G39" s="14">
+        <v>44968</v>
+      </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="5"/>
@@ -1436,9 +1469,15 @@
       <c r="D40" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="9"/>
+      <c r="E40" s="7">
+        <v>1</v>
+      </c>
+      <c r="F40" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="5"/>
@@ -1447,9 +1486,15 @@
       <c r="D41" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="9"/>
+      <c r="E41" s="7">
+        <v>1</v>
+      </c>
+      <c r="F41" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G41" s="14">
+        <v>44996</v>
+      </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="5"/>
@@ -1458,9 +1503,15 @@
       <c r="D42" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="9"/>
+      <c r="E42" s="7">
+        <v>1</v>
+      </c>
+      <c r="F42" s="7">
+        <v>1</v>
+      </c>
+      <c r="G42" s="14">
+        <v>45027</v>
+      </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="5"/>
@@ -1469,7 +1520,9 @@
       <c r="D43" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E43" s="7"/>
+      <c r="E43" s="7">
+        <v>2.5</v>
+      </c>
       <c r="F43" s="7"/>
       <c r="G43" s="9"/>
     </row>
@@ -1480,7 +1533,9 @@
       <c r="D44" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="7"/>
+      <c r="E44" s="7">
+        <v>2</v>
+      </c>
       <c r="F44" s="7"/>
       <c r="G44" s="9"/>
     </row>
@@ -1491,7 +1546,9 @@
       <c r="D45" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E45" s="7"/>
+      <c r="E45" s="7">
+        <v>1.5</v>
+      </c>
       <c r="F45" s="7"/>
       <c r="G45" s="9"/>
     </row>
@@ -1502,7 +1559,9 @@
       <c r="D46" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E46" s="7"/>
+      <c r="E46" s="7">
+        <v>2</v>
+      </c>
       <c r="F46" s="7"/>
       <c r="G46" s="9"/>
     </row>
@@ -1513,7 +1572,9 @@
       <c r="D47" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E47" s="7"/>
+      <c r="E47" s="7">
+        <v>1.5</v>
+      </c>
       <c r="F47" s="7"/>
       <c r="G47" s="9"/>
     </row>
@@ -1524,7 +1585,9 @@
       <c r="D48" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E48" s="7"/>
+      <c r="E48" s="7">
+        <v>1.5</v>
+      </c>
       <c r="F48" s="7"/>
       <c r="G48" s="9"/>
     </row>
@@ -1535,7 +1598,9 @@
       <c r="D49" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E49" s="7"/>
+      <c r="E49" s="7">
+        <v>3</v>
+      </c>
       <c r="F49" s="7"/>
       <c r="G49" s="9"/>
     </row>
@@ -1546,7 +1611,9 @@
       <c r="D50" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E50" s="7"/>
+      <c r="E50" s="7">
+        <v>3</v>
+      </c>
       <c r="F50" s="7"/>
       <c r="G50" s="9"/>
     </row>
@@ -1557,7 +1624,9 @@
       <c r="D51" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E51" s="7"/>
+      <c r="E51" s="7">
+        <v>3</v>
+      </c>
       <c r="F51" s="7"/>
       <c r="G51" s="9"/>
     </row>

</xml_diff>

<commit_message>
Final Assessment model of database completed
</commit_message>
<xml_diff>
--- a/API/API_BasicTraining.xlsx
+++ b/API/API_BasicTraining.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="109">
   <si>
     <t>No</t>
   </si>
@@ -358,6 +358,12 @@
   </si>
   <si>
     <t>8/11/2023 &amp; 20/11/2023</t>
+  </si>
+  <si>
+    <t>1-3-4/1/2024</t>
+  </si>
+  <si>
+    <t>1 + 1 + 3</t>
   </si>
 </sst>
 </file>
@@ -841,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1708,9 +1714,15 @@
         <v>62</v>
       </c>
       <c r="D54" s="18"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="9"/>
+      <c r="E54" s="7">
+        <v>8</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G54" s="14" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="5"/>

</xml_diff>